<commit_message>
Update grain orientation logic to use color codes
Changed from component-type-based to color-code-based grain assignment:

Grain rules by color:
- HS00, HS99, HS98, HS97 -> 'mixed' (can rotate 90 degrees)
- HS01, HS02, HS03 -> 'fixed' (cannot rotate)
- Other colors default to 'fixed'

Updated:
- generate_test_data.py: Grain assignment logic and docstring
- TEST_DATA_README.md: Documentation with color code table
- Regenerated test_data/ with new grain rules

This ensures components are correctly categorized for rotation
based on their actual material finish properties.
</commit_message>
<xml_diff>
--- a/test_data/wardrobe_order_001.xlsx
+++ b/test_data/wardrobe_order_001.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,12 +489,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>柜体侧板（R）</t>
+          <t>柜体侧板（L）</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CB(R)-HS00-2434-574-16</t>
+          <t>CB(L)-HS00-2434-574-16</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -516,19 +516,19 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>mixed</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>柜体侧板（L）</t>
+          <t>柜体侧板（R）</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CB(L)-HS00-2434-574-16</t>
+          <t>CB(R)-HS00-2434-574-16</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -550,23 +550,23 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>mixed</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>顶底板（单门柜体）</t>
+          <t>顶底板（双门柜体）</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>DD-HS00-368-554-16</t>
+          <t>DD-HS00-704-554-16</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>368</v>
+        <v>704</v>
       </c>
       <c r="D4" t="n">
         <v>554</v>
@@ -580,11 +580,11 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>mixed</t>
         </is>
       </c>
     </row>
@@ -596,11 +596,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DD-HS00-736-554-16</t>
+          <t>DD-HS00-896-554-16</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>736</v>
+        <v>896</v>
       </c>
       <c r="D5" t="n">
         <v>554</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -625,16 +625,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>顶底板（单门柜体）</t>
+          <t>顶底板（双门柜体）</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DD-HS00-432-554-16</t>
+          <t>DD-HS00-832-554-16</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>432</v>
+        <v>832</v>
       </c>
       <c r="D6" t="n">
         <v>554</v>
@@ -659,22 +659,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>层隔板（单门柜体）</t>
+          <t>顶底板（双门柜体）</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CG-HS00-432-554-25</t>
+          <t>DD-HS00-736-554-16</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>432</v>
+        <v>736</v>
       </c>
       <c r="D7" t="n">
         <v>554</v>
       </c>
       <c r="E7" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -698,11 +698,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CG-HS00-672-554-25</t>
+          <t>CG-HS00-896-554-25</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>672</v>
+        <v>896</v>
       </c>
       <c r="D8" t="n">
         <v>554</v>
@@ -716,27 +716,27 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>mixed</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>抽屉层隔板（E/F类柜体）与"抽屉组件"搭配使用</t>
+          <t>层隔板（双门柜体）</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CTCG-HS00-832-554-25</t>
+          <t>CG-HS00-704-554-25</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>832</v>
+        <v>704</v>
       </c>
       <c r="D9" t="n">
         <v>554</v>
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -761,16 +761,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>抽屉层隔板（E/F类柜体）与"抽屉组件"搭配使用</t>
+          <t>层隔板（单门柜体）</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CTCG-HS00-768-554-25</t>
+          <t>CG-HS00-336-554-25</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>768</v>
+        <v>336</v>
       </c>
       <c r="D10" t="n">
         <v>554</v>
@@ -784,33 +784,33 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>mixed</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>抽屉层隔板（E/F类柜体）与"抽屉组件"搭配使用</t>
+          <t>后背板（双门柜体）为(1+1)组合</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CTCG-HS00-704-554-25</t>
+          <t>HB-HS00-2320-464-12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>704</v>
+        <v>2320</v>
       </c>
       <c r="D11" t="n">
-        <v>554</v>
+        <v>464</v>
       </c>
       <c r="E11" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -822,29 +822,29 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>mixed</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>层隔板（双门柜体）</t>
+          <t>后背板（双门柜体）为(1+1)组合</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CG-HS00-800-554-25</t>
+          <t>HB-HS00-2256-336-12</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>800</v>
+        <v>2256</v>
       </c>
       <c r="D12" t="n">
-        <v>554</v>
+        <v>336</v>
       </c>
       <c r="E12" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -852,41 +852,41 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>mixed</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>抽屉层隔板（E/F类柜体）与"抽屉组件"搭配使用</t>
+          <t>门板（L/R）</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CTCG-HS00-896-554-25</t>
+          <t>MB(R)-(门板花色)-2320-397-16</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>896</v>
+        <v>2320</v>
       </c>
       <c r="D13" t="n">
-        <v>554</v>
+        <v>397</v>
       </c>
       <c r="E13" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>HS00</t>
+          <t>(门板花色)</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -897,34 +897,34 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>后背板（双门柜体）为(1+1)组合</t>
+          <t>门板（L/R）</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>HB-HS00-2288-432-12</t>
+          <t>MB(L)-(门板花色)-2288-397-16</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>2288</v>
       </c>
       <c r="D14" t="n">
-        <v>432</v>
+        <v>397</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>HS00</t>
+          <t>(门板花色)</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>mixed</t>
+          <t>fixed</t>
         </is>
       </c>
     </row>
@@ -936,14 +936,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MB(R)-(门板花色)-2256-381-16</t>
+          <t>MB(L)-(门板花色)-2320-397-16</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2256</v>
+        <v>2320</v>
       </c>
       <c r="D15" t="n">
-        <v>381</v>
+        <v>397</v>
       </c>
       <c r="E15" t="n">
         <v>16</v>
@@ -954,7 +954,7 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -965,60 +965,60 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>门板（L/R）</t>
+          <t>双抽屉组件</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MB(R)-(门板花色)-2352-461-16</t>
+          <t>CTF2抽屉吊板(R)-HS00-534-371-16</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2352</v>
+        <v>534</v>
       </c>
       <c r="D16" t="n">
-        <v>461</v>
+        <v>371</v>
       </c>
       <c r="E16" t="n">
         <v>16</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>(门板花色)</t>
+          <t>HS00</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>mixed</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>门板（L/R）</t>
+          <t>双抽屉组件</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MB(R)-(门板花色)-2352-445-16</t>
+          <t>抽屉拉板-HS00-438-106-12</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2352</v>
+        <v>438</v>
       </c>
       <c r="D17" t="n">
-        <v>445</v>
+        <v>106</v>
       </c>
       <c r="E17" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>(门板花色)</t>
+          <t>HS00</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>mixed</t>
         </is>
       </c>
     </row>
@@ -1038,17 +1038,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>526抽屉后板-HS00-526-138-12</t>
+          <t>800抽屉面板-HS00-800-170-16</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>526</v>
+        <v>800</v>
       </c>
       <c r="D18" t="n">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="E18" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1067,22 +1067,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>双抽屉组件</t>
+          <t>单抽屉组件</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>632抽屉底板-HS00-632-448-5</t>
+          <t>526抽屉后板-HS00-526-138-12</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>632</v>
+        <v>526</v>
       </c>
       <c r="D19" t="n">
-        <v>448</v>
+        <v>138</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1090,41 +1090,41 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>mixed</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>单抽屉组件</t>
+          <t>收口条</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>抽屉侧板(L)-HS00-450-138-12</t>
+          <t>TSB50-HS98-2434-50-16</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>450</v>
+        <v>2434</v>
       </c>
       <c r="D20" t="n">
-        <v>138</v>
+        <v>50</v>
       </c>
       <c r="E20" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>HS00</t>
+          <t>HS98</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1135,64 +1135,64 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>单抽屉组件</t>
+          <t>底支撑(双门柜体）</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>抽屉侧板(L)-HS00-450-138-12</t>
+          <t>DC-HS03-672-82-16</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>450</v>
+        <v>672</v>
       </c>
       <c r="D21" t="n">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="E21" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>HS00</t>
+          <t>HS03</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>mixed</t>
+          <t>fixed</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>圆弧衔接板</t>
+          <t>底支撑(双门柜体）</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>YX-HS99-2434-560-16</t>
+          <t>DC-HS97-832-82-16</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2434</v>
+        <v>832</v>
       </c>
       <c r="D22" t="n">
-        <v>560</v>
+        <v>82</v>
       </c>
       <c r="E22" t="n">
         <v>16</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>HS99</t>
+          <t>HS97</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1208,7 +1208,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>DC-HS03-368-82-16</t>
+          <t>DC-HS02-368-82-16</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1222,81 +1222,13 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>HS03</t>
+          <t>HS02</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23" t="inlineStr">
-        <is>
-          <t>mixed</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>底支撑(双门柜体）</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>DC-HS99-704-82-16</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>704</v>
-      </c>
-      <c r="D24" t="n">
-        <v>82</v>
-      </c>
-      <c r="E24" t="n">
-        <v>16</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>HS99</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
-        <v>2</v>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>fixed</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>收口条</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>TSA60-HS02-2434-60-16</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>2434</v>
-      </c>
-      <c r="D25" t="n">
-        <v>60</v>
-      </c>
-      <c r="E25" t="n">
-        <v>16</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>HS02</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25" t="inlineStr">
         <is>
           <t>fixed</t>
         </is>

</xml_diff>